<commit_message>
changes to temaplate and blade
</commit_message>
<xml_diff>
--- a/Projects/JNJUKTRIAL_SAND/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJUKTRIAL_SAND/Data/KPI Exclusions Template.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -79,6 +79,12 @@
     <t xml:space="preserve">Value3</t>
   </si>
   <si>
+    <t xml:space="preserve">Exclude4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value4</t>
+  </si>
+  <si>
     <t xml:space="preserve">All</t>
   </si>
   <si>
@@ -98,6 +104,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIGHT GUARD</t>
   </si>
 </sst>
 </file>
@@ -107,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -137,6 +149,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -220,7 +238,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,6 +265,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -326,22 +348,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.246963562753"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,28 +389,40 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="230.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jnjuk - exclude + kpi updates
</commit_message>
<xml_diff>
--- a/Projects/JNJUKTRIAL_SAND/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJUKTRIAL_SAND/Data/KPI Exclusions Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -73,43 +73,13 @@
     <t xml:space="preserve">Value2</t>
   </si>
   <si>
-    <t xml:space="preserve">Exclude3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exclude4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value4</t>
-  </si>
-  <si>
     <t xml:space="preserve">All</t>
   </si>
   <si>
-    <t xml:space="preserve">sub_category</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> COLD &amp; FLU; IBS; KIDS COLD &amp; FLU; KIDS COUGH;  KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH; KIDS HAYFEVER; LAXATIVES; KIDS TEETHING; WIND; Allergy; ANTI-AGE FACE; ARTIFICIAL TAN; BODY CLEANSING; Body Spray; COSMETICS; DEODORANTS; MEN'S TOILETRIES; Hair Care;  BABY HEALTHCARE; FOR MUM;KIDS HAIRCARE; KIDS TOILETRIES; KIDS WIPES; SANITARY TOWELS; SANITARY TOWELS; KIDS MOUTHWASH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary Shelf; Cooler; Chiller; POSM; Exterior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mixed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brand_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIGHT GUARD</t>
+    <t xml:space="preserve">Sub Category </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLD &amp; FLU ; IBS ; KIDS COLD &amp; FLU ; COLD &amp; FLU ;KIDS COUGH ; KIDS DECONGESTANTS ; KIDS DIGESTIVE HEALTH ; KIDS HAYFEVER ; LAXATIVES ; KIDS TEETHING ; WIND ; ALLERGY ; REHYDRATION ; PROBIOTICS ; PAIN MANAGEMENT ; ANTI-AGE FACE ; ARTIFICIAL TAN ; BODY CLEANSING ; BODY SPRAY ; COSMETICS ; DEODORANTS ; MEN'S TOILETRIES ; SUNCARE ; HAIR CARE ;  BABY HEALTHCARE ; FOR MUM ; KIDS HAIRCARE ; KIDS TOILETRIES ;  KIDS WIPES ; COTTON ; INCONTINENCE ; SANITARY TOWELS ; FEMININE WASH ; KIDS MOUTHWASH </t>
   </si>
 </sst>
 </file>
@@ -119,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -151,12 +121,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -172,7 +136,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,12 +159,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCC99FF"/>
         <bgColor rgb="FF9999FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF66CC"/>
-        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -238,7 +196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -255,20 +213,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -303,7 +253,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF66CC"/>
+      <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
@@ -348,23 +298,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.246963562753"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.0485829959514"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7732793522267"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.336032388664"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7287449392713"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,46 +330,16 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="247.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="230.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>